<commit_message>
Alterações para o documento final
</commit_message>
<xml_diff>
--- a/Algoritimos/Quadro Resumo Produtos.xlsx
+++ b/Algoritimos/Quadro Resumo Produtos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Documents\GitHub\projeto-de-graduacao\Algoritimos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EBD2C0-59E6-4DA0-B116-EDE7D62C282E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C205BB-36DD-44C3-ACB0-AE1DD0080667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="548" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,21 +17,22 @@
     <sheet name="Distribuições" sheetId="8" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="11" r:id="rId3"/>
     <sheet name="Dados consolidados" sheetId="10" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="12" r:id="rId5"/>
-    <sheet name="Quadro Nível de estoque" sheetId="6" state="hidden" r:id="rId6"/>
-    <sheet name="Quadro Ritmo de pedido" sheetId="7" state="hidden" r:id="rId7"/>
-    <sheet name="8864" sheetId="5" r:id="rId8"/>
-    <sheet name="697" sheetId="4" r:id="rId9"/>
-    <sheet name="8863" sheetId="3" r:id="rId10"/>
-    <sheet name="1972" sheetId="2" r:id="rId11"/>
+    <sheet name="Graficos projecao" sheetId="12" r:id="rId5"/>
+    <sheet name="Faltas" sheetId="13" r:id="rId6"/>
+    <sheet name="Quadro Nível de estoque" sheetId="6" state="hidden" r:id="rId7"/>
+    <sheet name="Quadro Ritmo de pedido" sheetId="7" state="hidden" r:id="rId8"/>
+    <sheet name="8864" sheetId="5" r:id="rId9"/>
+    <sheet name="697" sheetId="4" r:id="rId10"/>
+    <sheet name="8863" sheetId="3" r:id="rId11"/>
+    <sheet name="1972" sheetId="2" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
     <externalReference r:id="rId15"/>
     <externalReference r:id="rId16"/>
     <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -334,7 +335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="142">
   <si>
     <t>MATERIAL</t>
   </si>
@@ -655,9 +656,6 @@
     <t>RESULTADO CUSTO (t,s,S) (R$)</t>
   </si>
   <si>
-    <t>PERFORMACE (s,S) x (t,s,S)</t>
-  </si>
-  <si>
     <t>FTL - FULL TRUCK LOAD (KG)</t>
   </si>
   <si>
@@ -693,17 +691,90 @@
   <si>
     <t>[115.000, 205.000]</t>
   </si>
+  <si>
+    <t>[50, 350]</t>
+  </si>
+  <si>
+    <t>[60, 350]</t>
+  </si>
+  <si>
+    <t>[70, 350]</t>
+  </si>
+  <si>
+    <t>[80, 350]</t>
+  </si>
+  <si>
+    <t>[90, 350]</t>
+  </si>
+  <si>
+    <t>[100, 350]</t>
+  </si>
+  <si>
+    <t>[110, 350]</t>
+  </si>
+  <si>
+    <t>[120, 350]</t>
+  </si>
+  <si>
+    <t>[130, 350]</t>
+  </si>
+  <si>
+    <t>[140, 350]</t>
+  </si>
+  <si>
+    <t>Política</t>
+  </si>
+  <si>
+    <t>Custo Total</t>
+  </si>
+  <si>
+    <t>Custo Estoque</t>
+  </si>
+  <si>
+    <t>Custo Pedido</t>
+  </si>
+  <si>
+    <t>N Pedidos</t>
+  </si>
+  <si>
+    <t>N Faltas</t>
+  </si>
+  <si>
+    <t>PERFORMACE  (t,s,S) x (s,S)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> REDUÇÃO (%)</t>
+  </si>
+  <si>
+    <t>Nº  FALTAS POLÍTICA ATUAL (s,S)</t>
+  </si>
+  <si>
+    <t>Nº  FALTAS POLÍTICA ÓTIMIZADA (s,S)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nº  FALTAS EVITADAS </t>
+  </si>
+  <si>
+    <t>PERCENTUAL REDUZIDO (%)</t>
+  </si>
+  <si>
+    <t>Nº  FALTAS POLÍTICA ÓTIMIZADA (t,s,S)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,8 +844,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -799,8 +876,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -963,6 +1070,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -971,7 +1106,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1157,6 +1292,52 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1165,7 +1346,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="91">
+  <dxfs count="83">
     <dxf>
       <fill>
         <patternFill>
@@ -1231,65 +1412,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4991,7 +5113,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -18116,6 +18237,895 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Faltas!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N Pedidos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Faltas!$C$4:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>[50, 350]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[60, 350]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>[70, 350]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>[80, 350]</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>[90, 350]</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>[100, 350]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>[110, 350]</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>[120, 350]</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>[130, 350]</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>[140, 350]</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>[150, 350]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Faltas!$G$4:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E000-40DC-A042-94F11AF5E98E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="378942272"/>
+        <c:axId val="378942752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="378942272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Pol[itica</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> (s,S)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378942752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="378942752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Pedidos/ano</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378942272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Faltas!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N Faltas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Faltas!$C$4:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>[50, 350]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[60, 350]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>[70, 350]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>[80, 350]</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>[90, 350]</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>[100, 350]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>[110, 350]</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>[120, 350]</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>[130, 350]</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>[140, 350]</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>[150, 350]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Faltas!$H$4:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>33.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1013-4258-B984-4326E423259E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="378936992"/>
+        <c:axId val="378941312"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="378936992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378941312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="378941312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378936992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -18317,6 +19327,86 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -21452,6 +22542,1014 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -21687,6 +23785,83 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>150495</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>455295</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>122872</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC15754D-38B7-460F-BE96-FED253A29D23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>75247</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>94297</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{708BBDBF-D0DB-4525-B626-80AA70E05114}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -21778,7 +23953,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -21871,7 +24046,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -21920,7 +24095,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -39592,30 +41767,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83E7869D-2AD4-4626-B12C-E912772A2B93}" name="Table1" displayName="Table1" ref="C2:M9" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88" totalsRowBorderDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83E7869D-2AD4-4626-B12C-E912772A2B93}" name="Table1" displayName="Table1" ref="C2:M9" totalsRowShown="0" headerRowDxfId="82" headerRowBorderDxfId="81" tableBorderDxfId="80" totalsRowBorderDxfId="79">
   <autoFilter ref="C2:M9" xr:uid="{83E7869D-2AD4-4626-B12C-E912772A2B93}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D3:L5">
     <sortCondition ref="D2:D5"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="13" xr3:uid="{C3A53A4B-502B-4697-B076-E4F686CE67D1}" name="Material" dataDxfId="86"/>
-    <tableColumn id="1" xr3:uid="{D6FB5409-BB84-4BA2-A9C5-B205619445D7}" name="Código Material " dataDxfId="85"/>
-    <tableColumn id="10" xr3:uid="{C0A45B5B-AA8B-45AD-900E-926BD93D225D}" name="DISTRIBUIÇÃO DEMANDA" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{0617AC86-64A7-4CA5-9CBD-3E000DEA3E97}" name="LEAD TIME" dataDxfId="83"/>
-    <tableColumn id="4" xr3:uid="{ACD9A4C8-E495-41A2-9BC2-A11DE1A87D88}" name="POLÍTICA (s)" dataDxfId="82" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{C388735B-A43D-404A-9D09-34A3A1148B7D}" name="POLÍTICA (S)." dataDxfId="81"/>
-    <tableColumn id="6" xr3:uid="{A33D3C7B-6B85-462D-9BB9-DAAE82F28255}" name="PREÇO" dataDxfId="80"/>
-    <tableColumn id="7" xr3:uid="{31D13463-3F36-4A72-8B74-6F5F9129D735}" name="FTL - FULL TRUCK LOAD" dataDxfId="79"/>
-    <tableColumn id="8" xr3:uid="{863DD9A1-93D8-4CA6-AED9-EFA8EE89DC7E}" name="CUSTO ESTOQUE" dataDxfId="78"/>
-    <tableColumn id="9" xr3:uid="{2D8762ED-16BF-4D06-BB67-7AC4C5E58195}" name="CUSTO PEDIDO" dataDxfId="77"/>
-    <tableColumn id="11" xr3:uid="{F07B7160-023F-4FEB-B492-D2E489C1DF70}" name="Estoque Inical" dataDxfId="76"/>
+    <tableColumn id="13" xr3:uid="{C3A53A4B-502B-4697-B076-E4F686CE67D1}" name="Material" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{D6FB5409-BB84-4BA2-A9C5-B205619445D7}" name="Código Material " dataDxfId="77"/>
+    <tableColumn id="10" xr3:uid="{C0A45B5B-AA8B-45AD-900E-926BD93D225D}" name="DISTRIBUIÇÃO DEMANDA" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{0617AC86-64A7-4CA5-9CBD-3E000DEA3E97}" name="LEAD TIME" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{ACD9A4C8-E495-41A2-9BC2-A11DE1A87D88}" name="POLÍTICA (s)" dataDxfId="74" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{C388735B-A43D-404A-9D09-34A3A1148B7D}" name="POLÍTICA (S)." dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{A33D3C7B-6B85-462D-9BB9-DAAE82F28255}" name="PREÇO" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{31D13463-3F36-4A72-8B74-6F5F9129D735}" name="FTL - FULL TRUCK LOAD" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{863DD9A1-93D8-4CA6-AED9-EFA8EE89DC7E}" name="CUSTO ESTOQUE" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{2D8762ED-16BF-4D06-BB67-7AC4C5E58195}" name="CUSTO PEDIDO" dataDxfId="69"/>
+    <tableColumn id="11" xr3:uid="{F07B7160-023F-4FEB-B492-D2E489C1DF70}" name="Estoque Inical" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A55BAC89-7DDA-47B9-834E-42DEE256786E}" name="Table2" displayName="Table2" ref="F2:H9" totalsRowShown="0" headerRowDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A55BAC89-7DDA-47B9-834E-42DEE256786E}" name="Table2" displayName="Table2" ref="F2:H9" totalsRowShown="0" headerRowDxfId="67">
   <autoFilter ref="F2:H9" xr:uid="{A55BAC89-7DDA-47B9-834E-42DEE256786E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -39631,7 +41806,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7D6E9C37-8375-4E6B-A148-9F9C5C378B4B}" name="Table26" displayName="Table26" ref="B2:D9" totalsRowShown="0" headerRowDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7D6E9C37-8375-4E6B-A148-9F9C5C378B4B}" name="Table26" displayName="Table26" ref="B2:D9" totalsRowShown="0" headerRowDxfId="66">
   <autoFilter ref="B2:D9" xr:uid="{7D6E9C37-8375-4E6B-A148-9F9C5C378B4B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -39647,7 +41822,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{892F9641-2E20-4C88-8F96-D6EF5D2B719B}" name="Table10" displayName="Table10" ref="B15:J22" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{892F9641-2E20-4C88-8F96-D6EF5D2B719B}" name="Table10" displayName="Table10" ref="B15:J22" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62">
   <autoFilter ref="B15:J22" xr:uid="{892F9641-2E20-4C88-8F96-D6EF5D2B719B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -39660,22 +41835,22 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{1F951C20-3CFD-4959-A4E6-54FDB5196559}" name="MATERIAL" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{86ABB21F-3BA3-4763-8C79-5B98D81FBD92}" name="DISTRIBUIÇÃO DEMANDA" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{99F4005B-7B86-463B-9CFC-18C132A77416}" name="LEAD TIME" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{108722A6-54FB-4B5F-9AA7-7A1B31A239FF}" name="POLÍTICA (s,S)" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{D61FB745-C5D9-417C-BAA2-BEAB726E6D95}" name="PREÇO (R$)" dataDxfId="65" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{FF893F96-A67D-4C20-B532-D65A691C2C43}" name="FTL - FULL TRUCK LOAD (KG)" dataDxfId="64" dataCellStyle="Comma"/>
-    <tableColumn id="8" xr3:uid="{7D42886C-0C60-4E9D-9639-61A1084F8F97}" name="CUSTO ESTOQUE" dataDxfId="63" dataCellStyle="Percent"/>
-    <tableColumn id="9" xr3:uid="{BC96E7D2-179A-45B0-AABC-0230DD7F0DC7}" name="CUSTO PEDIDO" dataDxfId="62" dataCellStyle="Currency"/>
-    <tableColumn id="10" xr3:uid="{CA185293-5C45-4017-A62B-392C27E7154E}" name="ESTOQUE INICIAL" dataDxfId="61" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{1F951C20-3CFD-4959-A4E6-54FDB5196559}" name="MATERIAL" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{86ABB21F-3BA3-4763-8C79-5B98D81FBD92}" name="DISTRIBUIÇÃO DEMANDA" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{99F4005B-7B86-463B-9CFC-18C132A77416}" name="LEAD TIME" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{108722A6-54FB-4B5F-9AA7-7A1B31A239FF}" name="POLÍTICA (s,S)" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{D61FB745-C5D9-417C-BAA2-BEAB726E6D95}" name="PREÇO (R$)" dataDxfId="57" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{FF893F96-A67D-4C20-B532-D65A691C2C43}" name="FTL - FULL TRUCK LOAD (KG)" dataDxfId="56" dataCellStyle="Comma"/>
+    <tableColumn id="8" xr3:uid="{7D42886C-0C60-4E9D-9639-61A1084F8F97}" name="CUSTO ESTOQUE" dataDxfId="55" dataCellStyle="Percent"/>
+    <tableColumn id="9" xr3:uid="{BC96E7D2-179A-45B0-AABC-0230DD7F0DC7}" name="CUSTO PEDIDO" dataDxfId="54" dataCellStyle="Currency"/>
+    <tableColumn id="10" xr3:uid="{CA185293-5C45-4017-A62B-392C27E7154E}" name="ESTOQUE INICIAL" dataDxfId="53" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F714A836-3B69-4329-9840-26B39652ED13}" name="Table105" displayName="Table105" ref="D4:L11" totalsRowShown="0" headerRowDxfId="60" dataDxfId="58" headerRowBorderDxfId="59" tableBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F714A836-3B69-4329-9840-26B39652ED13}" name="Table105" displayName="Table105" ref="D4:L11" totalsRowShown="0" headerRowDxfId="52" dataDxfId="50" headerRowBorderDxfId="51" tableBorderDxfId="49">
   <autoFilter ref="D4:L11" xr:uid="{F714A836-3B69-4329-9840-26B39652ED13}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -39688,22 +41863,22 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{338ABB0F-3FC1-47AB-9774-8A5905501DC1}" name="MATERIAL" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{6B5C589C-5674-407D-A8E6-FBCACA2842D3}" name="DISTRIBUIÇÃO DEMANDA" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{5B7AE21E-FABF-4553-A09A-4D8A302E451A}" name="LEAD TIME" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{2CA77A7C-080D-40C7-AE84-1CC96A4941C1}" name="POLÍTICA (s,S)" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{0AC07981-AA60-46DE-89A2-1C4C97E95129}" name="PREÇO (R$)" dataDxfId="52" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{754BA6A5-44AE-44FF-BB22-A8AAAB5CDA60}" name="FTL - FULL TRUCK LOAD (KG)" dataDxfId="51" dataCellStyle="Comma"/>
-    <tableColumn id="8" xr3:uid="{1A779E17-2146-4FD4-A906-000DAE19A216}" name="CUSTO ESTOQUE" dataDxfId="50" dataCellStyle="Percent"/>
-    <tableColumn id="9" xr3:uid="{4CF93AD8-3063-423D-9DB5-4C21A9CC73A5}" name="CUSTO PEDIDO" dataDxfId="49" dataCellStyle="Currency"/>
-    <tableColumn id="10" xr3:uid="{F13E885A-BC98-4981-975D-4BE955C8EAD8}" name="ESTOQUE INICIAL" dataDxfId="48" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{338ABB0F-3FC1-47AB-9774-8A5905501DC1}" name="MATERIAL" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{6B5C589C-5674-407D-A8E6-FBCACA2842D3}" name="DISTRIBUIÇÃO DEMANDA" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{5B7AE21E-FABF-4553-A09A-4D8A302E451A}" name="LEAD TIME" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{2CA77A7C-080D-40C7-AE84-1CC96A4941C1}" name="POLÍTICA (s,S)" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{0AC07981-AA60-46DE-89A2-1C4C97E95129}" name="PREÇO (R$)" dataDxfId="44" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{754BA6A5-44AE-44FF-BB22-A8AAAB5CDA60}" name="FTL - FULL TRUCK LOAD (KG)" dataDxfId="43" dataCellStyle="Comma"/>
+    <tableColumn id="8" xr3:uid="{1A779E17-2146-4FD4-A906-000DAE19A216}" name="CUSTO ESTOQUE" dataDxfId="42" dataCellStyle="Percent"/>
+    <tableColumn id="9" xr3:uid="{4CF93AD8-3063-423D-9DB5-4C21A9CC73A5}" name="CUSTO PEDIDO" dataDxfId="41" dataCellStyle="Currency"/>
+    <tableColumn id="10" xr3:uid="{F13E885A-BC98-4981-975D-4BE955C8EAD8}" name="ESTOQUE INICIAL" dataDxfId="40" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{573A128F-E7BF-4449-BA1F-1AA0DE83758C}" name="Table17" displayName="Table17" ref="B2:J9" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{573A128F-E7BF-4449-BA1F-1AA0DE83758C}" name="Table17" displayName="Table17" ref="B2:J9" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <autoFilter ref="B2:J9" xr:uid="{573A128F-E7BF-4449-BA1F-1AA0DE83758C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -39719,17 +41894,17 @@
     <sortCondition ref="B2:B5"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="13" xr3:uid="{5734E4A9-D82B-43FC-9D2A-EA0E3268A21C}" name="MATERIAL" dataDxfId="43"/>
-    <tableColumn id="10" xr3:uid="{A854BCA7-4EF0-4922-8EAC-C5F980FAED66}" name="POLÍTICA ATUAL (s,S)" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{920E6275-EE39-4602-B5A1-CD9F6D3F9692}" name="CUSTO TOTAL  (R$)" dataDxfId="41" dataCellStyle="Currency"/>
-    <tableColumn id="1" xr3:uid="{77AA2BD1-BA49-46B1-84F4-CE5458B54E09}" name="Nº  FALTAS" dataDxfId="40" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{D6B88208-3BA0-4DA2-80BA-F03724F5FD44}" name="POLÍTICA OTIMIZADA (s,S)" dataDxfId="39" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{62368DA7-1173-4740-B374-62DF7B615C82}" name="CUSTO MINIMIZADO (R$) " dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{B73F4C3E-F128-4A60-953C-3812D0EC9709}" name="Nº FALTAS MIN" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{175CA05E-6C0B-4E4B-86EC-A8698A047907}" name="RESULTADO CUSTO (R$)" dataDxfId="36" dataCellStyle="Currency">
+    <tableColumn id="13" xr3:uid="{5734E4A9-D82B-43FC-9D2A-EA0E3268A21C}" name="MATERIAL" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{A854BCA7-4EF0-4922-8EAC-C5F980FAED66}" name="POLÍTICA ATUAL (s,S)" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{920E6275-EE39-4602-B5A1-CD9F6D3F9692}" name="CUSTO TOTAL  (R$)" dataDxfId="33" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{77AA2BD1-BA49-46B1-84F4-CE5458B54E09}" name="Nº  FALTAS" dataDxfId="32" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{D6B88208-3BA0-4DA2-80BA-F03724F5FD44}" name="POLÍTICA OTIMIZADA (s,S)" dataDxfId="31" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{62368DA7-1173-4740-B374-62DF7B615C82}" name="CUSTO MINIMIZADO (R$) " dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{B73F4C3E-F128-4A60-953C-3812D0EC9709}" name="Nº FALTAS MIN" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{175CA05E-6C0B-4E4B-86EC-A8698A047907}" name="RESULTADO CUSTO (R$)" dataDxfId="28" dataCellStyle="Currency">
       <calculatedColumnFormula>D3-G3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3810F6CC-65CB-496B-9FCC-B42FED92B992}" name="(%)" dataDxfId="35" dataCellStyle="Percent">
+    <tableColumn id="7" xr3:uid="{3810F6CC-65CB-496B-9FCC-B42FED92B992}" name="(%)" dataDxfId="27" dataCellStyle="Percent">
       <calculatedColumnFormula>Table17[[#This Row],[RESULTADO CUSTO (R$)]]/Table17[[#This Row],[CUSTO TOTAL  (R$)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -39738,7 +41913,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FA201908-0471-484D-9420-43E7B83E69F0}" name="Table174" displayName="Table174" ref="B13:J20" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FA201908-0471-484D-9420-43E7B83E69F0}" name="Table174" displayName="Table174" ref="B13:J20" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="B13:J20" xr:uid="{FA201908-0471-484D-9420-43E7B83E69F0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -39754,21 +41929,21 @@
     <sortCondition ref="B2:B5"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="13" xr3:uid="{81E4783D-7264-4C46-BD7A-A1446801B0A2}" name="MATERIAL" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{A49CC638-13F1-4512-B7C3-E3931BB81AEA}" name="POLÍTICA ATUAL (s,S)" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{F0D3ACD7-4707-4D8B-A6BD-B9044248596F}" name="CUSTO TOTAL (R$)" dataDxfId="28">
+    <tableColumn id="13" xr3:uid="{81E4783D-7264-4C46-BD7A-A1446801B0A2}" name="MATERIAL" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{A49CC638-13F1-4512-B7C3-E3931BB81AEA}" name="POLÍTICA ATUAL (s,S)" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{F0D3ACD7-4707-4D8B-A6BD-B9044248596F}" name="CUSTO TOTAL (R$)" dataDxfId="20">
       <calculatedColumnFormula>D3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{8E5BC272-191E-4891-8117-37C7C3C32566}" name="Nº  FALTAS" dataDxfId="27" dataCellStyle="Currency">
+    <tableColumn id="1" xr3:uid="{8E5BC272-191E-4891-8117-37C7C3C32566}" name="Nº  FALTAS" dataDxfId="19" dataCellStyle="Currency">
       <calculatedColumnFormula>E3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{969D7873-F12E-4C5E-95ED-E4964BA60825}" name="POLÍTICA OTIMIZADA (t,s,S)" dataDxfId="26" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{021FEB45-1A66-4480-A964-33DE128D3240}" name="CUSTO MINIMIZADO (R$) " dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{6D304835-6205-42BF-A098-BD62C8241DEB}" name="Nº FALTAS MIN" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{F4BFCF29-A46C-4F50-823E-3BF219DF36FD}" name="RESULTADO CUSTO (R$)" dataDxfId="23" dataCellStyle="Currency">
+    <tableColumn id="4" xr3:uid="{969D7873-F12E-4C5E-95ED-E4964BA60825}" name="POLÍTICA OTIMIZADA (t,s,S)" dataDxfId="18" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{021FEB45-1A66-4480-A964-33DE128D3240}" name="CUSTO MINIMIZADO (R$) " dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{6D304835-6205-42BF-A098-BD62C8241DEB}" name="Nº FALTAS MIN" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{F4BFCF29-A46C-4F50-823E-3BF219DF36FD}" name="RESULTADO CUSTO (R$)" dataDxfId="15" dataCellStyle="Currency">
       <calculatedColumnFormula>D14-G14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{81293E98-C2F5-4194-A1D8-C786F1A0B667}" name="(%)" dataDxfId="22" dataCellStyle="Percent">
+    <tableColumn id="7" xr3:uid="{81293E98-C2F5-4194-A1D8-C786F1A0B667}" name="(%)" dataDxfId="14" dataCellStyle="Percent">
       <calculatedColumnFormula>Table174[[#This Row],[RESULTADO CUSTO (R$)]]/Table174[[#This Row],[CUSTO TOTAL (R$)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -40042,7 +42217,7 @@
   <dimension ref="A2:M17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40410,60 +42585,32 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A15:A17">
+    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="Não Simulado">
+      <formula>NOT(ISERROR(SEARCH("Não Simulado",A15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="2" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",A15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="Em Simulação">
+      <formula>NOT(ISERROR(SEARCH("Em Simulação",A15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Simulado">
+      <formula>NOT(ISERROR(SEARCH("Simulado",A15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A3:B9">
-    <cfRule type="containsText" dxfId="21" priority="17" operator="containsText" text="Não Simulado">
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Não Simulado">
       <formula>NOT(ISERROR(SEARCH("Não Simulado",A3)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="18" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Em Simulação">
+    <cfRule type="containsText" dxfId="9" priority="19" operator="containsText" text="Em Simulação">
       <formula>NOT(ISERROR(SEARCH("Em Simulação",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Simulado">
+    <cfRule type="containsText" dxfId="8" priority="20" operator="containsText" text="Simulado">
       <formula>NOT(ISERROR(SEARCH("Simulado",A3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Não Simulado">
-      <formula>NOT(ISERROR(SEARCH("Não Simulado",A15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="10" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",A15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="Em Simulação">
-      <formula>NOT(ISERROR(SEARCH("Em Simulação",A15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="Simulado">
-      <formula>NOT(ISERROR(SEARCH("Simulado",A15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="Não Simulado">
-      <formula>NOT(ISERROR(SEARCH("Não Simulado",A16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="6" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",A16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="Em Simulação">
-      <formula>NOT(ISERROR(SEARCH("Em Simulação",A16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Simulado">
-      <formula>NOT(ISERROR(SEARCH("Simulado",A16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="Não Simulado">
-      <formula>NOT(ISERROR(SEARCH("Não Simulado",A17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="2" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",A17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Em Simulação">
-      <formula>NOT(ISERROR(SEARCH("Em Simulação",A17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Simulado">
-      <formula>NOT(ISERROR(SEARCH("Simulado",A17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -40481,6 +42628,27 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBC540C-4C98-4727-89C3-A206D76411A6}">
+  <dimension ref="O1"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P54" sqref="P54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1582E92-05CB-476A-B2B2-2A68D9D30B96}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -40495,7 +42663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014675F7-AFAE-41B2-A6F6-5779A43A74EC}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -40708,7 +42876,7 @@
         <v>70</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>4</v>
@@ -40731,7 +42899,7 @@
         <v>21</v>
       </c>
       <c r="E16" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F16" s="44" t="s">
         <v>6</v>
@@ -40972,7 +43140,7 @@
         <v>70</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>4</v>
@@ -41197,10 +43365,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA629734-46C6-4C91-BDEA-F36A23B0CA4D}">
-  <dimension ref="B2:W35"/>
+  <dimension ref="B2:AC49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF27" sqref="AF27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41208,26 +43376,32 @@
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" customWidth="1"/>
     <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.109375" customWidth="1"/>
     <col min="11" max="11" width="15.5546875" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" customWidth="1"/>
     <col min="13" max="13" width="28.33203125" customWidth="1"/>
-    <col min="14" max="14" width="20.33203125" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" customWidth="1"/>
+    <col min="14" max="14" width="28" customWidth="1"/>
+    <col min="15" max="15" width="14.77734375" customWidth="1"/>
     <col min="16" max="16" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.5546875" customWidth="1"/>
     <col min="20" max="20" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.77734375" customWidth="1"/>
     <col min="22" max="22" width="12.44140625" customWidth="1"/>
+    <col min="23" max="23" width="10.88671875" customWidth="1"/>
+    <col min="25" max="25" width="12" customWidth="1"/>
+    <col min="26" max="26" width="15.109375" customWidth="1"/>
+    <col min="27" max="27" width="17.5546875" customWidth="1"/>
+    <col min="28" max="28" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:29" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -41283,15 +43457,30 @@
         <v>104</v>
       </c>
       <c r="W2" s="61" t="s">
-        <v>86</v>
+        <v>136</v>
+      </c>
+      <c r="Y2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA2" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB2" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC2" s="60" t="s">
+        <v>140</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B3" s="37" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="48">
         <v>14001975.722468469</v>
@@ -41300,7 +43489,7 @@
         <v>33</v>
       </c>
       <c r="F3" s="42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G3" s="48">
         <v>13519723.49029321</v>
@@ -41322,7 +43511,7 @@
       <c r="M3" s="48">
         <v>482252.23217525892</v>
       </c>
-      <c r="N3" s="49">
+      <c r="N3" s="84">
         <f>Table17[[#This Row],[RESULTADO CUSTO (R$)]]/Table17[[#This Row],[CUSTO TOTAL  (R$)]]</f>
         <v>3.4441727491457227E-2</v>
       </c>
@@ -41349,8 +43538,24 @@
         <f>V3/S3</f>
         <v>0.5757575757575758</v>
       </c>
+      <c r="Y3" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z3" s="58">
+        <v>33</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>14</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC3" s="93">
+        <f>AB3/Z3</f>
+        <v>0.5757575757575758</v>
+      </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B4" s="37" t="s">
         <v>58</v>
       </c>
@@ -41364,7 +43569,7 @@
         <v>253</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G4" s="48">
         <v>12139296.40254201</v>
@@ -41386,7 +43591,7 @@
       <c r="M4" s="48">
         <v>117962.8690295592</v>
       </c>
-      <c r="N4" s="49">
+      <c r="N4" s="84">
         <f>Table17[[#This Row],[RESULTADO CUSTO (R$)]]/Table17[[#This Row],[CUSTO TOTAL  (R$)]]</f>
         <v>9.6239188888785372E-3</v>
       </c>
@@ -41413,8 +43618,24 @@
         <f t="shared" ref="W4:W9" si="2">V4/S4</f>
         <v>2.766798418972332E-2</v>
       </c>
+      <c r="Y4" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z4" s="58">
+        <v>253</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>246</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>7</v>
+      </c>
+      <c r="AC4" s="93">
+        <f t="shared" ref="AC4:AC10" si="3">AB4/Z4</f>
+        <v>2.766798418972332E-2</v>
+      </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B5" s="37" t="s">
         <v>59</v>
       </c>
@@ -41428,7 +43649,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G5" s="48">
         <v>4074935.978300618</v>
@@ -41450,7 +43671,7 @@
       <c r="M5" s="48">
         <v>158847.24010927789</v>
       </c>
-      <c r="N5" s="49">
+      <c r="N5" s="84">
         <f>Table17[[#This Row],[RESULTADO CUSTO (R$)]]/Table17[[#This Row],[CUSTO TOTAL  (R$)]]</f>
         <v>3.7518982884753596E-2</v>
       </c>
@@ -41477,8 +43698,24 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
+      <c r="Y5" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z5" s="58">
+        <v>12</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>9</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="93">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B6" s="37" t="s">
         <v>60</v>
       </c>
@@ -41514,7 +43751,7 @@
       <c r="M6" s="54">
         <v>85809.98991697398</v>
       </c>
-      <c r="N6" s="49">
+      <c r="N6" s="84">
         <f>Table17[[#This Row],[RESULTADO CUSTO (R$)]]/Table17[[#This Row],[CUSTO TOTAL  (R$)]]</f>
         <v>6.1533651316581922E-2</v>
       </c>
@@ -41541,8 +43778,24 @@
         <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
+      <c r="Y6" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z6" s="58">
+        <v>15</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>12</v>
+      </c>
+      <c r="AC6" s="93">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B7" s="37" t="s">
         <v>61</v>
       </c>
@@ -41578,7 +43831,7 @@
       <c r="M7" s="48">
         <v>631296.47458354011</v>
       </c>
-      <c r="N7" s="49">
+      <c r="N7" s="84">
         <f>Table17[[#This Row],[RESULTADO CUSTO (R$)]]/Table17[[#This Row],[CUSTO TOTAL  (R$)]]</f>
         <v>2.3559806680680886E-2</v>
       </c>
@@ -41605,8 +43858,24 @@
         <f t="shared" si="2"/>
         <v>9.2105263157894732E-2</v>
       </c>
+      <c r="Y7" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z7" s="58">
+        <v>76</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>69</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>7</v>
+      </c>
+      <c r="AC7" s="93">
+        <f t="shared" si="3"/>
+        <v>9.2105263157894732E-2</v>
+      </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B8" s="37" t="s">
         <v>62</v>
       </c>
@@ -41620,7 +43889,7 @@
         <v>37</v>
       </c>
       <c r="F8" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G8" s="48">
         <v>6430311.863330842</v>
@@ -41642,7 +43911,7 @@
       <c r="M8" s="48">
         <v>2550580.1966691585</v>
       </c>
-      <c r="N8" s="49">
+      <c r="N8" s="84">
         <f>Table17[[#This Row],[RESULTADO CUSTO (R$)]]/Table17[[#This Row],[CUSTO TOTAL  (R$)]]</f>
         <v>0.28400076291187026</v>
       </c>
@@ -41669,8 +43938,24 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="Y8" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z8" s="58">
+        <v>37</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC8" s="93">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B9" s="37" t="s">
         <v>63</v>
       </c>
@@ -41706,7 +43991,7 @@
       <c r="M9" s="48">
         <v>73777.969669777289</v>
       </c>
-      <c r="N9" s="49">
+      <c r="N9" s="84">
         <f>Table17[[#This Row],[RESULTADO CUSTO (R$)]]/Table17[[#This Row],[CUSTO TOTAL  (R$)]]</f>
         <v>0.42816921210215042</v>
       </c>
@@ -41733,8 +44018,24 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="Y9" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z9" s="58">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="93">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:29" x14ac:dyDescent="0.3">
       <c r="L10" s="55" t="s">
         <v>102</v>
       </c>
@@ -41742,15 +44043,37 @@
         <f>SUM(M3:M9)</f>
         <v>4100526.9721535458</v>
       </c>
-      <c r="V10" s="27"/>
+      <c r="V10" s="86">
+        <f>SUM(V3:V9)</f>
+        <v>86</v>
+      </c>
+      <c r="Y10" s="89" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z10" s="90">
+        <f>SUM(Z3:Z9)</f>
+        <v>427</v>
+      </c>
+      <c r="AA10" s="91">
+        <f>SUM(AA3:AA9)</f>
+        <v>341</v>
+      </c>
+      <c r="AB10" s="92">
+        <f>SUM(AB3:AB9)</f>
+        <v>86</v>
+      </c>
+      <c r="AC10" s="94">
+        <f t="shared" si="3"/>
+        <v>0.20140515222482436</v>
+      </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:29" x14ac:dyDescent="0.3">
       <c r="V11" s="27"/>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:29" x14ac:dyDescent="0.3">
       <c r="V12" s="27"/>
     </row>
-    <row r="13" spans="2:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>0</v>
       </c>
@@ -41806,15 +44129,30 @@
         <v>104</v>
       </c>
       <c r="W13" s="61" t="s">
-        <v>86</v>
+        <v>136</v>
+      </c>
+      <c r="Y13" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA13" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB13" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC13" s="60" t="s">
+        <v>140</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B14" s="37" t="s">
         <v>57</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D14" s="51">
         <f>D3</f>
@@ -41825,7 +44163,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G14" s="48">
         <v>13391947.13412741</v>
@@ -41847,7 +44185,7 @@
       <c r="M14" s="48">
         <v>610028.58834105916</v>
       </c>
-      <c r="N14" s="49">
+      <c r="N14" s="84">
         <f>M14/Table174[[#This Row],[CUSTO TOTAL (R$)]]</f>
         <v>4.3567322243115172E-2</v>
       </c>
@@ -41874,8 +44212,24 @@
         <f>V14/S14</f>
         <v>0.5757575757575758</v>
       </c>
+      <c r="Y14" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z14" s="58">
+        <v>33</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>14</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC14" s="93">
+        <f>AB14/Z14</f>
+        <v>0.5757575757575758</v>
+      </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B15" s="37" t="s">
         <v>58</v>
       </c>
@@ -41883,15 +44237,15 @@
         <v>72</v>
       </c>
       <c r="D15" s="51">
-        <f t="shared" ref="D15:E20" si="3">D4</f>
+        <f t="shared" ref="D15:E20" si="4">D4</f>
         <v>12257259.271571569</v>
       </c>
       <c r="E15" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>253</v>
       </c>
       <c r="F15" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G15" s="48">
         <v>12166184.025861099</v>
@@ -41900,7 +44254,7 @@
         <v>245</v>
       </c>
       <c r="I15" s="48">
-        <f t="shared" ref="I15:I20" si="4">D15-G15</f>
+        <f t="shared" ref="I15:I20" si="5">D15-G15</f>
         <v>91075.245710469782</v>
       </c>
       <c r="J15" s="49">
@@ -41913,7 +44267,7 @@
       <c r="M15" s="48">
         <v>91075.245710469782</v>
       </c>
-      <c r="N15" s="49">
+      <c r="N15" s="84">
         <f>M15/Table174[[#This Row],[CUSTO TOTAL (R$)]]</f>
         <v>7.4303107809509956E-3</v>
       </c>
@@ -41933,15 +44287,31 @@
         <v>245</v>
       </c>
       <c r="V15" s="64">
-        <f t="shared" ref="V15:V20" si="5">S15-U15</f>
+        <f t="shared" ref="V15:V20" si="6">S15-U15</f>
         <v>8</v>
       </c>
       <c r="W15" s="62">
-        <f t="shared" ref="W15:W20" si="6">V15/S15</f>
+        <f t="shared" ref="W15:W21" si="7">V15/S15</f>
         <v>3.1620553359683792E-2</v>
       </c>
+      <c r="Y15" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z15" s="58">
+        <v>253</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>245</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>8</v>
+      </c>
+      <c r="AC15" s="93">
+        <f t="shared" ref="AC15:AC21" si="8">AB15/Z15</f>
+        <v>3.1620553359683792E-2</v>
+      </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B16" s="37" t="s">
         <v>59</v>
       </c>
@@ -41949,15 +44319,15 @@
         <v>73</v>
       </c>
       <c r="D16" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4233783.2184098959</v>
       </c>
       <c r="E16" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G16" s="48">
         <v>4000996.643078865</v>
@@ -41979,7 +44349,7 @@
       <c r="M16" s="48">
         <v>232786.57533103088</v>
       </c>
-      <c r="N16" s="49">
+      <c r="N16" s="84">
         <f>M16/Table174[[#This Row],[CUSTO TOTAL (R$)]]</f>
         <v>5.4983111633774145E-2</v>
       </c>
@@ -41999,15 +44369,31 @@
         <v>5</v>
       </c>
       <c r="V16" s="64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="W16" s="62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.58333333333333337</v>
       </c>
+      <c r="Y16" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z16" s="58">
+        <v>12</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>7</v>
+      </c>
+      <c r="AC16" s="93">
+        <f t="shared" si="8"/>
+        <v>0.58333333333333337</v>
+      </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B17" s="37" t="s">
         <v>60</v>
       </c>
@@ -42015,7 +44401,7 @@
         <v>74</v>
       </c>
       <c r="D17" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1394521.3404531081</v>
       </c>
       <c r="E17" s="52">
@@ -42023,7 +44409,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G17" s="48">
         <v>1286873.992347064</v>
@@ -42032,7 +44418,7 @@
         <v>3</v>
       </c>
       <c r="I17" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>107647.34810604411</v>
       </c>
       <c r="J17" s="49">
@@ -42045,7 +44431,7 @@
       <c r="M17" s="54">
         <v>107647.34810604411</v>
       </c>
-      <c r="N17" s="49">
+      <c r="N17" s="84">
         <f>M17/Table174[[#This Row],[CUSTO TOTAL (R$)]]</f>
         <v>7.7193044655069473E-2</v>
       </c>
@@ -42065,15 +44451,31 @@
         <v>3</v>
       </c>
       <c r="V17" s="64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="W17" s="62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.8</v>
       </c>
+      <c r="Y17" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z17" s="58">
+        <v>15</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>12</v>
+      </c>
+      <c r="AC17" s="93">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B18" s="37" t="s">
         <v>61</v>
       </c>
@@ -42081,7 +44483,7 @@
         <v>75</v>
       </c>
       <c r="D18" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26795486.191370372</v>
       </c>
       <c r="E18" s="50">
@@ -42089,7 +44491,7 @@
         <v>76</v>
       </c>
       <c r="F18" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G18" s="48">
         <v>25826297.36561133</v>
@@ -42111,7 +44513,7 @@
       <c r="M18" s="48">
         <v>969188.82575904205</v>
       </c>
-      <c r="N18" s="49">
+      <c r="N18" s="84">
         <f>M18/Table174[[#This Row],[CUSTO TOTAL (R$)]]</f>
         <v>3.6169854088005854E-2</v>
       </c>
@@ -42131,15 +44533,31 @@
         <v>66</v>
       </c>
       <c r="V18" s="64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="W18" s="62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.13157894736842105</v>
       </c>
+      <c r="Y18" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z18" s="58">
+        <v>76</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>66</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>10</v>
+      </c>
+      <c r="AC18" s="93">
+        <f t="shared" si="8"/>
+        <v>0.13157894736842105</v>
+      </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B19" s="37" t="s">
         <v>62</v>
       </c>
@@ -42147,15 +44565,15 @@
         <v>76</v>
       </c>
       <c r="D19" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8980892.0600000005</v>
       </c>
       <c r="E19" s="50">
-        <f t="shared" ref="E19" si="7">E8</f>
+        <f t="shared" ref="E19" si="9">E8</f>
         <v>37</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G19" s="51">
         <v>6034554.8990950799</v>
@@ -42164,7 +44582,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2946337.1609049207</v>
       </c>
       <c r="J19" s="49">
@@ -42177,7 +44595,7 @@
       <c r="M19" s="48">
         <v>2946337.1609049207</v>
       </c>
-      <c r="N19" s="49">
+      <c r="N19" s="84">
         <f>M19/Table174[[#This Row],[CUSTO TOTAL (R$)]]</f>
         <v>0.32806731683455065</v>
       </c>
@@ -42197,15 +44615,31 @@
         <v>0</v>
       </c>
       <c r="V19" s="64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="W19" s="62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
+      <c r="Y19" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z19" s="58">
+        <v>37</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC19" s="93">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B20" s="37" t="s">
         <v>63</v>
       </c>
@@ -42213,11 +44647,11 @@
         <v>77</v>
       </c>
       <c r="D20" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>172310.31</v>
       </c>
       <c r="E20" s="50">
-        <f t="shared" ref="E20" si="8">E9</f>
+        <f t="shared" ref="E20" si="10">E9</f>
         <v>1</v>
       </c>
       <c r="F20" s="42" t="s">
@@ -42230,7 +44664,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>78158.850543236258</v>
       </c>
       <c r="J20" s="49">
@@ -42243,7 +44677,7 @@
       <c r="M20" s="48">
         <v>78158.850543236258</v>
       </c>
-      <c r="N20" s="49">
+      <c r="N20" s="84">
         <f>M20/Table174[[#This Row],[CUSTO TOTAL (R$)]]</f>
         <v>0.45359358092522878</v>
       </c>
@@ -42263,15 +44697,31 @@
         <v>0</v>
       </c>
       <c r="V20" s="64">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="W20" s="62">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
+      <c r="W20" s="62">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y20" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z20" s="58">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="93">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:29" x14ac:dyDescent="0.3">
       <c r="L21" s="55" t="s">
         <v>102</v>
       </c>
@@ -42279,160 +44729,638 @@
         <f>SUM(M14:M20)</f>
         <v>5035222.5946958028</v>
       </c>
+      <c r="R21" s="87" t="s">
+        <v>135</v>
+      </c>
+      <c r="S21" s="1">
+        <f>SUM(S14:S20)</f>
+        <v>427</v>
+      </c>
+      <c r="U21" s="87" t="s">
+        <v>135</v>
+      </c>
+      <c r="V21" s="88">
+        <f>SUM(V14:V20)</f>
+        <v>94</v>
+      </c>
+      <c r="W21" s="62">
+        <f t="shared" si="7"/>
+        <v>0.22014051522248243</v>
+      </c>
+      <c r="Y21" s="89" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z21" s="90">
+        <f>SUM(Z14:Z20)</f>
+        <v>427</v>
+      </c>
+      <c r="AA21" s="91">
+        <f>SUM(AA14:AA20)</f>
+        <v>333</v>
+      </c>
+      <c r="AB21" s="92">
+        <f>SUM(AB14:AB20)</f>
+        <v>94</v>
+      </c>
+      <c r="AC21" s="94">
+        <f t="shared" si="8"/>
+        <v>0.22014051522248243</v>
+      </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="D24" s="70"/>
+    </row>
+    <row r="25" spans="2:29" x14ac:dyDescent="0.3">
       <c r="D25" s="70"/>
+      <c r="U25">
+        <f>V21/S21</f>
+        <v>0.22014051522248243</v>
+      </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D26" s="70"/>
+    <row r="26" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="D26" s="85"/>
       <c r="G26" s="72"/>
+      <c r="U26">
+        <f>V10/S21</f>
+        <v>0.20140515222482436</v>
+      </c>
     </row>
-    <row r="27" spans="2:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:29" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L27" s="16" t="s">
         <v>0</v>
       </c>
       <c r="M27" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="N27" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="N27" s="16" t="s">
+      <c r="O27" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="R27" t="s">
         <v>105</v>
       </c>
-      <c r="O27" s="16" t="s">
-        <v>106</v>
-      </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:29" x14ac:dyDescent="0.3">
       <c r="L28" s="53" t="s">
         <v>57</v>
       </c>
       <c r="M28" s="48">
+        <v>610028.58834105916</v>
+      </c>
+      <c r="N28" s="48">
         <v>482252.23217525892</v>
       </c>
-      <c r="N28" s="48">
+      <c r="O28" s="63">
+        <f>M28 -N28</f>
+        <v>127776.35616580024</v>
+      </c>
+      <c r="R28">
         <v>610028.58834105916</v>
       </c>
-      <c r="O28" s="63">
-        <f>N28 -M28</f>
-        <v>127776.35616580024</v>
-      </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:29" x14ac:dyDescent="0.3">
       <c r="L29" s="53" t="s">
         <v>58</v>
       </c>
       <c r="M29" s="48">
+        <v>91075.245710469782</v>
+      </c>
+      <c r="N29" s="48">
         <v>117962.8690295592</v>
       </c>
-      <c r="N29" s="48">
+      <c r="O29" s="63">
+        <f t="shared" ref="O29:O34" si="11">M29 -N29</f>
+        <v>-26887.623319089413</v>
+      </c>
+      <c r="R29">
         <v>91075.245710469782</v>
       </c>
-      <c r="O29" s="63">
-        <f t="shared" ref="O29:O34" si="9">N29 -M29</f>
-        <v>-26887.623319089413</v>
-      </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:29" x14ac:dyDescent="0.3">
       <c r="L30" s="53" t="s">
         <v>59</v>
       </c>
       <c r="M30" s="48">
+        <v>232786.57533103088</v>
+      </c>
+      <c r="N30" s="48">
         <v>158847.24010927789</v>
       </c>
-      <c r="N30" s="48">
+      <c r="O30" s="63">
+        <f t="shared" si="11"/>
+        <v>73939.33522175299</v>
+      </c>
+      <c r="R30">
         <v>232786.57533103088</v>
       </c>
-      <c r="O30" s="63">
-        <f t="shared" si="9"/>
-        <v>73939.33522175299</v>
-      </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="H31" s="61" t="s">
+        <v>86</v>
+      </c>
       <c r="L31" s="53" t="s">
         <v>60</v>
       </c>
       <c r="M31" s="54">
+        <v>107647.34810604411</v>
+      </c>
+      <c r="N31" s="54">
         <v>85809.98991697398</v>
       </c>
-      <c r="N31" s="54">
+      <c r="O31" s="63">
+        <f t="shared" si="11"/>
+        <v>21837.358189070132</v>
+      </c>
+      <c r="R31">
         <v>107647.34810604411</v>
       </c>
-      <c r="O31" s="63">
-        <f t="shared" si="9"/>
-        <v>21837.358189070132</v>
-      </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B32" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="58">
+        <v>33</v>
+      </c>
+      <c r="E32" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="2">
+        <v>14</v>
+      </c>
+      <c r="G32" s="64">
+        <v>19</v>
+      </c>
+      <c r="H32" s="62">
+        <f>G32/D32</f>
+        <v>0.5757575757575758</v>
+      </c>
       <c r="L32" s="53" t="s">
         <v>61</v>
       </c>
       <c r="M32" s="48">
+        <v>969188.82575904205</v>
+      </c>
+      <c r="N32" s="48">
         <v>631296.47458354011</v>
       </c>
-      <c r="N32" s="48">
+      <c r="O32" s="63">
+        <f t="shared" si="11"/>
+        <v>337892.35117550194</v>
+      </c>
+      <c r="R32">
         <v>969188.82575904205</v>
       </c>
-      <c r="O32" s="63">
-        <f t="shared" si="9"/>
-        <v>337892.35117550194</v>
-      </c>
     </row>
-    <row r="33" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B33" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="58">
+        <v>253</v>
+      </c>
+      <c r="E33" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="2">
+        <v>246</v>
+      </c>
+      <c r="G33" s="64">
+        <v>7</v>
+      </c>
+      <c r="H33" s="62">
+        <f t="shared" ref="H33:H38" si="12">G33/D33</f>
+        <v>2.766798418972332E-2</v>
+      </c>
       <c r="L33" s="53" t="s">
         <v>62</v>
       </c>
       <c r="M33" s="48">
+        <v>2946337.1609049207</v>
+      </c>
+      <c r="N33" s="48">
         <v>2550580.1966691585</v>
       </c>
-      <c r="N33" s="48">
+      <c r="O33" s="63">
+        <f t="shared" si="11"/>
+        <v>395756.96423576213</v>
+      </c>
+      <c r="R33">
         <v>2946337.1609049207</v>
       </c>
-      <c r="O33" s="63">
-        <f t="shared" si="9"/>
-        <v>395756.96423576213</v>
-      </c>
     </row>
-    <row r="34" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B34" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="58">
+        <v>12</v>
+      </c>
+      <c r="E34" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" s="2">
+        <v>9</v>
+      </c>
+      <c r="G34" s="64">
+        <v>3</v>
+      </c>
+      <c r="H34" s="62">
+        <f t="shared" si="12"/>
+        <v>0.25</v>
+      </c>
       <c r="L34" s="53" t="s">
         <v>63</v>
       </c>
       <c r="M34" s="48">
+        <v>78158.850543236258</v>
+      </c>
+      <c r="N34" s="48">
         <v>73777.969669777289</v>
       </c>
-      <c r="N34" s="48">
+      <c r="O34" s="63">
+        <f t="shared" si="11"/>
+        <v>4380.8808734589693</v>
+      </c>
+      <c r="R34">
         <v>78158.850543236258</v>
       </c>
-      <c r="O34" s="63">
-        <f t="shared" si="9"/>
-        <v>4380.8808734589693</v>
-      </c>
     </row>
-    <row r="35" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B35" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="58">
+        <v>15</v>
+      </c>
+      <c r="E35" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="2">
+        <v>3</v>
+      </c>
+      <c r="G35" s="64">
+        <v>12</v>
+      </c>
+      <c r="H35" s="62">
+        <f t="shared" si="12"/>
+        <v>0.8</v>
+      </c>
       <c r="L35" s="55" t="s">
         <v>102</v>
       </c>
       <c r="M35" s="56">
-        <f>SUM(M28:M34)</f>
-        <v>4100526.9721535458</v>
+        <v>5035222.5946958028</v>
       </c>
       <c r="N35" s="56">
         <f>SUM(N28:N34)</f>
+        <v>4100526.9721535458</v>
+      </c>
+      <c r="O35" s="65">
+        <f>M35 -N35</f>
+        <v>934695.62254225696</v>
+      </c>
+      <c r="R35">
         <v>5035222.5946958028</v>
       </c>
-      <c r="O35" s="65">
-        <f>N35 -M35</f>
-        <v>934695.62254225696</v>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B36" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="58">
+        <v>76</v>
+      </c>
+      <c r="E36" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="2">
+        <v>69</v>
+      </c>
+      <c r="G36" s="64">
+        <v>7</v>
+      </c>
+      <c r="H36" s="62">
+        <f t="shared" si="12"/>
+        <v>9.2105263157894732E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B37" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="58">
+        <v>37</v>
+      </c>
+      <c r="E37" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="64">
+        <v>37</v>
+      </c>
+      <c r="H37" s="62">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B38" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="58">
+        <v>1</v>
+      </c>
+      <c r="E38" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="64">
+        <v>1</v>
+      </c>
+      <c r="H38" s="62">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G39" s="27"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G40" s="27"/>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G41" s="27"/>
+    </row>
+    <row r="42" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B42" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G42" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="H42" s="61" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B43" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="58">
+        <v>33</v>
+      </c>
+      <c r="E43" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="F43" s="2">
+        <v>14</v>
+      </c>
+      <c r="G43" s="64">
+        <f>D43-F43</f>
+        <v>19</v>
+      </c>
+      <c r="H43" s="62">
+        <f>G43/D43</f>
+        <v>0.5757575757575758</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B44" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="58">
+        <v>253</v>
+      </c>
+      <c r="E44" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" s="2">
+        <v>245</v>
+      </c>
+      <c r="G44" s="64">
+        <f t="shared" ref="G44:G49" si="13">D44-F44</f>
+        <v>8</v>
+      </c>
+      <c r="H44" s="62">
+        <f t="shared" ref="H44:H49" si="14">G44/D44</f>
+        <v>3.1620553359683792E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B45" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="58">
+        <v>12</v>
+      </c>
+      <c r="E45" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="F45" s="2">
+        <v>5</v>
+      </c>
+      <c r="G45" s="64">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="H45" s="62">
+        <f t="shared" si="14"/>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B46" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="58">
+        <v>15</v>
+      </c>
+      <c r="E46" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" s="2">
+        <v>3</v>
+      </c>
+      <c r="G46" s="64">
+        <f t="shared" si="13"/>
+        <v>12</v>
+      </c>
+      <c r="H46" s="62">
+        <f t="shared" si="14"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B47" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="58">
+        <v>76</v>
+      </c>
+      <c r="E47" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="F47" s="2">
+        <v>66</v>
+      </c>
+      <c r="G47" s="64">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="H47" s="62">
+        <f t="shared" si="14"/>
+        <v>0.13157894736842105</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B48" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="58">
+        <v>37</v>
+      </c>
+      <c r="E48" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0</v>
+      </c>
+      <c r="G48" s="64">
+        <f t="shared" si="13"/>
+        <v>37</v>
+      </c>
+      <c r="H48" s="62">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="58">
+        <v>1</v>
+      </c>
+      <c r="E49" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0</v>
+      </c>
+      <c r="G49" s="64">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="H49" s="62">
+        <f t="shared" si="14"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="M3:N9 M10">
-    <cfRule type="cellIs" dxfId="9" priority="16" operator="lessThan">
+  <conditionalFormatting sqref="M28:M35">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="&quot;&gt; 0&quot;"/>
+        <cfvo type="num" val="&quot;&lt; 0&quot;"/>
+        <color theme="9"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="18">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:N9 M10">
+    <cfRule type="cellIs" dxfId="5" priority="20" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="&quot;&gt; 0&quot;"/>
         <cfvo type="num" val="&quot;&lt; 0&quot;"/>
@@ -42442,29 +45370,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14:N20 M21">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="num" val="&quot;&gt; 0&quot;"/>
-        <cfvo type="num" val="&quot;&lt; 0&quot;"/>
-        <color theme="9"/>
-        <color rgb="FFC00000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M28:M35">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="num" val="&quot;&gt; 0&quot;"/>
         <cfvo type="num" val="&quot;&lt; 0&quot;"/>
@@ -42474,13 +45386,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28:N35">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="&quot;&gt; 0&quot;"/>
         <cfvo type="num" val="&quot;&lt; 0&quot;"/>
@@ -42489,14 +45395,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O28:O35">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="N28:O35">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="3">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O28:O35">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="&quot;&gt; 0&quot;"/>
         <cfvo type="num" val="&quot;&lt; 0&quot;"/>
@@ -42519,7 +45427,7 @@
   <dimension ref="B1:C1"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+      <selection activeCell="X3" sqref="X3:AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42538,6 +45446,270 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0361931-94A5-426A-B2AB-8333C8D8B163}">
+  <dimension ref="C2:H14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C3" s="82" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="83" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="83" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="82" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" s="82" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C4" s="73" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="74">
+        <v>86317.555108439861</v>
+      </c>
+      <c r="E4" s="74">
+        <v>77017.555108439861</v>
+      </c>
+      <c r="F4" s="74">
+        <v>9300</v>
+      </c>
+      <c r="G4" s="75">
+        <v>3</v>
+      </c>
+      <c r="H4" s="75">
+        <v>33.43</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C5" s="76" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="77">
+        <v>87154.535771138981</v>
+      </c>
+      <c r="E5" s="77">
+        <v>77854.535771138966</v>
+      </c>
+      <c r="F5" s="77">
+        <v>9300</v>
+      </c>
+      <c r="G5" s="78">
+        <v>3</v>
+      </c>
+      <c r="H5" s="78">
+        <v>26.78</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C6" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="74">
+        <v>87875.1882410322</v>
+      </c>
+      <c r="E6" s="74">
+        <v>78296.1882410322</v>
+      </c>
+      <c r="F6" s="74">
+        <v>9579</v>
+      </c>
+      <c r="G6" s="75">
+        <v>3.09</v>
+      </c>
+      <c r="H6" s="75">
+        <v>19.53</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="76" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="77">
+        <v>89033.486711053978</v>
+      </c>
+      <c r="E7" s="77">
+        <v>77563.486711053993</v>
+      </c>
+      <c r="F7" s="77">
+        <v>11470</v>
+      </c>
+      <c r="G7" s="78">
+        <v>3.7</v>
+      </c>
+      <c r="H7" s="78">
+        <v>14.74</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="79" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="80">
+        <v>89503.288743496581</v>
+      </c>
+      <c r="E8" s="80">
+        <v>77196.288743496581</v>
+      </c>
+      <c r="F8" s="80">
+        <v>12307</v>
+      </c>
+      <c r="G8" s="81">
+        <v>3.97</v>
+      </c>
+      <c r="H8" s="81">
+        <v>10.97</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="74">
+        <v>90694.168623749109</v>
+      </c>
+      <c r="E9" s="74">
+        <v>78294.168623749079</v>
+      </c>
+      <c r="F9" s="74">
+        <v>12400</v>
+      </c>
+      <c r="G9" s="75">
+        <v>4</v>
+      </c>
+      <c r="H9" s="75">
+        <v>6.17</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="76" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="77">
+        <v>91789.61250928542</v>
+      </c>
+      <c r="E10" s="77">
+        <v>79327.61250928542</v>
+      </c>
+      <c r="F10" s="77">
+        <v>12462</v>
+      </c>
+      <c r="G10" s="78">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="H10" s="78">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="74">
+        <v>93541.698309047802</v>
+      </c>
+      <c r="E11" s="74">
+        <v>79839.698309047773</v>
+      </c>
+      <c r="F11" s="74">
+        <v>13702</v>
+      </c>
+      <c r="G11" s="75">
+        <v>4.42</v>
+      </c>
+      <c r="H11" s="75">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="76" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="77">
+        <v>95910.7953531206</v>
+      </c>
+      <c r="E12" s="77">
+        <v>80472.7953531206</v>
+      </c>
+      <c r="F12" s="77">
+        <v>15438</v>
+      </c>
+      <c r="G12" s="78">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="H12" s="78">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="74">
+        <v>97034.188641164073</v>
+      </c>
+      <c r="E13" s="74">
+        <v>81534.188641164044</v>
+      </c>
+      <c r="F13" s="74">
+        <v>15500</v>
+      </c>
+      <c r="G13" s="75">
+        <v>5</v>
+      </c>
+      <c r="H13" s="75">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="77">
+        <v>98532.340330222709</v>
+      </c>
+      <c r="E14" s="77">
+        <v>83032.340330222723</v>
+      </c>
+      <c r="F14" s="77">
+        <v>15500</v>
+      </c>
+      <c r="G14" s="78">
+        <v>5</v>
+      </c>
+      <c r="H14" s="78">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2758A156-9043-4A24-BAD9-8DF23409CDDA}">
   <dimension ref="C2:E5"/>
   <sheetViews>
@@ -42592,7 +45764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC13200C-CE94-45E3-AA7D-CA0F07B853F4}">
   <dimension ref="B3:D7"/>
   <sheetViews>
@@ -42667,7 +45839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64943658-6A1B-43A4-93C7-5D3731F2B8D2}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -42680,25 +45852,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBC540C-4C98-4727-89C3-A206D76411A6}">
-  <dimension ref="O1"/>
-  <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P54" sqref="P54"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>